<commit_message>
Modify on Jul 9
</commit_message>
<xml_diff>
--- a/Universities_Programs.xlsx
+++ b/Universities_Programs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB2883E-9906-42C5-AEAF-99CECD543A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +17,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +33,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -48,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +89,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -108,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +120,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -139,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +151,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -170,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C26" authorId="0">
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -181,12 +182,12 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">作者:
+          <t xml:space="preserve">Author:
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -197,7 +198,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -217,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -227,7 +228,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -244,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -252,47 +253,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>4U English or French, depending on the language of instruction at your school
-4U Calculus and Vectors
-4U Physics
-4U Chemistry</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -310,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -321,34 +285,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-4U English or French, depending on the language of instruction at your school;
-4U Calculus and Vectors;
-Two of 4U Biology, Chemistry or Physics</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F32" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -366,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -374,10 +311,65 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+4U English or French, depending on the language of instruction at your school;
+4U Calculus and Vectors;
+Two of 4U Biology, Chemistry or Physics</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+4U English or French, depending on the language of instruction at your school
+4U Calculus and Vectors
+4U Physics
+4U Chemistry</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -749,18 +741,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -784,7 +776,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -792,7 +784,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -850,17 +842,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -868,12 +860,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -915,7 +910,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -948,9 +943,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -983,6 +995,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1158,25 +1187,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1196,8 +1225,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:7" ht="25.5" customHeight="1">
+      <c r="B3" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1216,8 +1245,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="7"/>
+    <row r="4" spans="2:7" ht="30" customHeight="1">
+      <c r="B4" s="8"/>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1234,8 +1263,8 @@
         <v>350</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B5" s="7"/>
+    <row r="5" spans="2:7" ht="28.8">
+      <c r="B5" s="8"/>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1252,8 +1281,8 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B6" s="7"/>
+    <row r="6" spans="2:7" ht="28.8">
+      <c r="B6" s="8"/>
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1270,8 +1299,8 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B7" s="7"/>
+    <row r="7" spans="2:7" ht="28.8">
+      <c r="B7" s="8"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1288,8 +1317,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B8" s="7"/>
+    <row r="8" spans="2:7" ht="28.8">
+      <c r="B8" s="8"/>
       <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1306,12 +1335,12 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:7">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="2:7" ht="28.8">
+      <c r="B10" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1330,8 +1359,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B11" s="7"/>
+    <row r="11" spans="2:7" ht="28.8">
+      <c r="B11" s="8"/>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
@@ -1348,8 +1377,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="81" x14ac:dyDescent="0.15">
-      <c r="B12" s="7"/>
+    <row r="12" spans="2:7" ht="72">
+      <c r="B12" s="8"/>
       <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
@@ -1366,8 +1395,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="81" x14ac:dyDescent="0.15">
-      <c r="B13" s="7"/>
+    <row r="13" spans="2:7" ht="72">
+      <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1384,12 +1413,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:7">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="2:7" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="2:7" ht="43.2">
+      <c r="B15" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1408,8 +1437,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B16" s="8"/>
+    <row r="16" spans="2:7" ht="28.8">
+      <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1426,11 +1455,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7">
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="43.2">
       <c r="B18" s="6" t="s">
         <v>52</v>
       </c>
@@ -1450,12 +1479,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B20" s="9" t="s">
+    <row r="20" spans="2:7" ht="28.8">
+      <c r="B20" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1471,8 +1500,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B21" s="9"/>
+    <row r="21" spans="2:7" ht="28.8">
+      <c r="B21" s="7"/>
       <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
@@ -1486,8 +1515,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="9"/>
+    <row r="22" spans="2:7" ht="18" customHeight="1">
+      <c r="B22" s="7"/>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
@@ -1501,11 +1530,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B24" s="9" t="s">
+    <row r="24" spans="2:7" ht="28.8">
+      <c r="B24" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1524,8 +1553,8 @@
         <v>345</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B25" s="9"/>
+    <row r="25" spans="2:7" ht="28.8">
+      <c r="B25" s="7"/>
       <c r="C25" s="2" t="s">
         <v>71</v>
       </c>
@@ -1542,8 +1571,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B26" s="9"/>
+    <row r="26" spans="2:7" ht="28.8">
+      <c r="B26" s="7"/>
       <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
@@ -1560,11 +1589,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7">
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B28" s="9" t="s">
+    <row r="28" spans="2:7">
+      <c r="B28" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1575,8 +1604,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B29" s="9"/>
+    <row r="29" spans="2:7">
+      <c r="B29" s="7"/>
       <c r="C29" s="2" t="s">
         <v>79</v>
       </c>
@@ -1587,8 +1616,8 @@
         <v>96.7</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="9"/>
+    <row r="30" spans="2:7" ht="21.75" customHeight="1">
+      <c r="B30" s="7"/>
       <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1599,8 +1628,8 @@
         <v>95.6</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="B31" s="9"/>
+    <row r="31" spans="2:7">
+      <c r="B31" s="7"/>
       <c r="C31" s="2" t="s">
         <v>82</v>
       </c>
@@ -1611,8 +1640,8 @@
         <v>92.8</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B32" s="9"/>
+    <row r="32" spans="2:7">
+      <c r="B32" s="7"/>
       <c r="C32" s="2" t="s">
         <v>83</v>
       </c>
@@ -1623,11 +1652,11 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:6">
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="2:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="B34" s="9" t="s">
+    <row r="34" spans="2:6" ht="28.8">
+      <c r="B34" s="7" t="s">
         <v>86</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -1635,29 +1664,29 @@
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B35" s="9"/>
+    <row r="35" spans="2:6">
+      <c r="B35" s="7"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B36" s="9"/>
+    <row r="36" spans="2:6">
+      <c r="B36" s="7"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B37" s="9"/>
+    <row r="37" spans="2:6">
+      <c r="B37" s="7"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B38" s="9"/>
+    <row r="38" spans="2:6">
+      <c r="B38" s="7"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:6">
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:6">
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:6">
       <c r="D41" s="3"/>
     </row>
   </sheetData>
@@ -1678,12 +1707,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1691,12 +1720,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>